<commit_message>
Código y actualización tabla
</commit_message>
<xml_diff>
--- a/Proyecto.xlsx
+++ b/Proyecto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Uni\Microcontroladores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Obsidian Vault\PROJECTS\Proyecto Microcontroladores\maceta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9156F1E6-C2AA-46CE-98B9-CF95E0B311AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E644CEA-291D-4A17-A0DF-6F1BA48A934B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D1E6F369-666C-497F-A044-47A35C75F709}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">Descripción </t>
   </si>
@@ -81,9 +81,6 @@
 (viene en el pack)</t>
   </si>
   <si>
-    <t>LDR</t>
-  </si>
-  <si>
     <t>MQ135</t>
   </si>
   <si>
@@ -112,17 +109,6 @@
     <t xml:space="preserve">Luminosidad </t>
   </si>
   <si>
-    <t>Sensor Pasivo</t>
-  </si>
-  <si>
-    <t>Resistencia de 10k</t>
-  </si>
-  <si>
-    <t>D33
-3V3
-GND</t>
-  </si>
-  <si>
     <t>Bomba de Agua</t>
   </si>
   <si>
@@ -137,6 +123,17 @@
   <si>
     <t>IN D23
 VIN
+GND</t>
+  </si>
+  <si>
+    <t>KY-018</t>
+  </si>
+  <si>
+    <t>Sensor Activo</t>
+  </si>
+  <si>
+    <t>D22
+3V3
 GND</t>
   </si>
 </sst>
@@ -555,7 +552,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,13 +603,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -620,16 +617,16 @@
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -637,36 +634,36 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>